<commit_message>
Adds note to schematic about 3.3V regulator option
</commit_message>
<xml_diff>
--- a/PBJ_EU/bom/Digi-Key/PBJ_EU.xlsx
+++ b/PBJ_EU/bom/Digi-Key/PBJ_EU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shann\Dropbox\moog\PBJ\PBJ_EU\bom\Digi-Key\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{466189F5-051F-482D-97CB-BC8322C952F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919E21DA-B742-4081-A40F-90D369E75B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBJ_EU" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1087,7 +1087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1096,6 +1096,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="44.140625" customWidth="1"/>
   </cols>

</xml_diff>